<commit_message>
unificando java e front
</commit_message>
<xml_diff>
--- a/outros/iniciandoTCC.xlsx
+++ b/outros/iniciandoTCC.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55">
   <si>
     <t>medicamento</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>cep</t>
+  </si>
+  <si>
+    <t>nome:String</t>
   </si>
   <si>
     <t>endereco_fk</t>
@@ -183,12 +186,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,16 +221,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,10 +283,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -271,99 +299,67 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -390,49 +386,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,127 +560,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,21 +589,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -622,6 +603,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,6 +654,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -666,166 +671,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -839,9 +835,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1162,7 +1155,7 @@
   <dimension ref="A1:AE11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1241,13 +1234,13 @@
       <c r="G2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" t="s">
         <v>18</v>
       </c>
       <c r="O2" t="s">
@@ -1291,13 +1284,13 @@
       <c r="G3" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" t="s">
         <v>24</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M3" t="s">
         <v>24</v>
       </c>
       <c r="O3" t="s">
@@ -1368,76 +1361,79 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="3:27">
+    <row r="6" spans="1:27">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="Y6" t="s">
         <v>14</v>
       </c>
-      <c r="AA6" s="5" t="s">
+      <c r="AA6" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:27">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
         <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Y7" t="s">
         <v>15</v>
       </c>
-      <c r="AA7" s="5" t="s">
-        <v>41</v>
+      <c r="AA7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:27">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AA8" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>